<commit_message>
Created Data Quality report. Also created a report mentioning handling missing values and outliers in variables, feature transaformation and new feature creation
</commit_message>
<xml_diff>
--- a/Data Quality Report/data_quality_report.xlsx
+++ b/Data Quality Report/data_quality_report.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gangu\OneDrive\Desktop\Academics\Data Science 1.0 Year 2020-2022\Lending club analysis\Data Quality Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gangu\OneDrive\Desktop\Academics\Lending club analysis\Data Quality Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{377BE500-8BAC-4DD2-87E3-2BA48C256959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5FC246-9886-4490-BBBD-AD0D8D59CAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data Quality Report" sheetId="1" r:id="rId1"/>
+    <sheet name="Version_control" sheetId="2" r:id="rId1"/>
+    <sheet name="Data Quality Report" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="184">
   <si>
     <t>Columns</t>
   </si>
@@ -543,13 +544,60 @@
   </si>
   <si>
     <t>Sr No</t>
+  </si>
+  <si>
+    <t>Report Name</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>data_quality_report</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Generates a report with the below data points:
+1. Missing value %
+2. Number of Unique values
+3. Data Types
+4. Descriptive statistical measures
+5. Type of distribution</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Model Developer</t>
+  </si>
+  <si>
+    <t>Souvik Ganguly</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>DQ reported submitted for approval</t>
+  </si>
+  <si>
+    <t>Model Owner- Approver 1</t>
+  </si>
+  <si>
+    <t>Model Sponsor- Approver 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -565,16 +613,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -582,15 +644,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -940,10 +1023,97 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{455AA3CF-7F11-4EF3-860A-762A1CFDF0B9}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="37.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D5" s="5">
+        <v>45416</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N152"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>